<commit_message>
modulo de aprobar empresas egresados
</commit_message>
<xml_diff>
--- a/TAEE/web/resources/files/Plantilla-Empresa.xlsx
+++ b/TAEE/web/resources/files/Plantilla-Empresa.xlsx
@@ -68,9 +68,6 @@
     <t>CONV019293</t>
   </si>
   <si>
-    <t>UPS7172636</t>
-  </si>
-  <si>
     <t>Grupo salinas</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>salinas.e@gmail.com</t>
+  </si>
+  <si>
+    <t>UPS7172639</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +565,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="2">
-        <v>566576</v>
+        <v>50000</v>
       </c>
       <c r="F2" s="2">
         <v>5566778899</v>
@@ -574,24 +574,24 @@
         <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2">
         <v>57888</v>
@@ -600,27 +600,27 @@
         <v>555565435</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="I3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2">
         <v>67888</v>
@@ -629,27 +629,27 @@
         <v>45366789</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="I4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E5" s="2">
         <v>5466577</v>
@@ -658,27 +658,27 @@
         <v>5566442233</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="I5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E6" s="2">
         <v>5454646</v>
@@ -687,22 +687,22 @@
         <v>67577383</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="I6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>

</xml_diff>